<commit_message>
small scale 1 Box configuration data
</commit_message>
<xml_diff>
--- a/Config/Calibrations/OneFifth1BoxCals with interpolated shunt cals.xlsx
+++ b/Config/Calibrations/OneFifth1BoxCals with interpolated shunt cals.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="15195" windowHeight="11760" firstSheet="2" activeTab="4"/>
@@ -886,11 +886,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149467904"/>
-        <c:axId val="149469824"/>
+        <c:axId val="84372288"/>
+        <c:axId val="84372864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149467904"/>
+        <c:axId val="84372288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,12 +964,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149469824"/>
+        <c:crossAx val="84372864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149469824"/>
+        <c:axId val="84372864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1053,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149467904"/>
+        <c:crossAx val="84372288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1319,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160656384"/>
-        <c:axId val="160674944"/>
+        <c:axId val="132660544"/>
+        <c:axId val="132988928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160656384"/>
+        <c:axId val="132660544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,12 +1397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160674944"/>
+        <c:crossAx val="132988928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160674944"/>
+        <c:axId val="132988928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160656384"/>
+        <c:crossAx val="132660544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1773,11 +1773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160958336"/>
-        <c:axId val="160972800"/>
+        <c:axId val="132990656"/>
+        <c:axId val="132991232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160958336"/>
+        <c:axId val="132990656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,12 +1851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160972800"/>
+        <c:crossAx val="132991232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160972800"/>
+        <c:axId val="132991232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160958336"/>
+        <c:crossAx val="132990656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2215,11 +2215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160989952"/>
-        <c:axId val="160991872"/>
+        <c:axId val="132992960"/>
+        <c:axId val="132993536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160989952"/>
+        <c:axId val="132992960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,12 +2293,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160991872"/>
+        <c:crossAx val="132993536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160991872"/>
+        <c:axId val="132993536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2382,7 +2382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160989952"/>
+        <c:crossAx val="132992960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2747,11 +2747,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161096448"/>
-        <c:axId val="161098368"/>
+        <c:axId val="132996416"/>
+        <c:axId val="132939776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161096448"/>
+        <c:axId val="132996416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2825,12 +2825,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161098368"/>
+        <c:crossAx val="132939776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161098368"/>
+        <c:axId val="132939776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2914,7 +2914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161096448"/>
+        <c:crossAx val="132996416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,11 +3231,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161127040"/>
-        <c:axId val="161129216"/>
+        <c:axId val="132995840"/>
+        <c:axId val="132995264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161127040"/>
+        <c:axId val="132995840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3309,12 +3309,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161129216"/>
+        <c:crossAx val="132995264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161129216"/>
+        <c:axId val="132995264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3398,7 +3398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161127040"/>
+        <c:crossAx val="132995840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3712,11 +3712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161158656"/>
-        <c:axId val="161160576"/>
+        <c:axId val="132942656"/>
+        <c:axId val="132943232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161158656"/>
+        <c:axId val="132942656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3790,12 +3790,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161160576"/>
+        <c:crossAx val="132943232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161160576"/>
+        <c:axId val="132943232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3879,7 +3879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161158656"/>
+        <c:crossAx val="132942656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4181,11 +4181,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161186176"/>
-        <c:axId val="161188096"/>
+        <c:axId val="132944960"/>
+        <c:axId val="132945536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161186176"/>
+        <c:axId val="132944960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4259,12 +4259,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161188096"/>
+        <c:crossAx val="132945536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161188096"/>
+        <c:axId val="132945536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4348,7 +4348,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161186176"/>
+        <c:crossAx val="132944960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4650,11 +4650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161225728"/>
-        <c:axId val="161236096"/>
+        <c:axId val="132947264"/>
+        <c:axId val="130981888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161225728"/>
+        <c:axId val="132947264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4728,12 +4728,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161236096"/>
+        <c:crossAx val="130981888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161236096"/>
+        <c:axId val="130981888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4817,7 +4817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161225728"/>
+        <c:crossAx val="132947264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5119,11 +5119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161273728"/>
-        <c:axId val="161275904"/>
+        <c:axId val="130983616"/>
+        <c:axId val="130984192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161273728"/>
+        <c:axId val="130983616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5197,12 +5197,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161275904"/>
+        <c:crossAx val="130984192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161275904"/>
+        <c:axId val="130984192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5286,7 +5286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161273728"/>
+        <c:crossAx val="130983616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5582,11 +5582,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="151947904"/>
-        <c:axId val="154285184"/>
+        <c:axId val="84374592"/>
+        <c:axId val="84375168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151947904"/>
+        <c:axId val="84374592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5660,12 +5660,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154285184"/>
+        <c:crossAx val="84375168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154285184"/>
+        <c:axId val="84375168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5749,7 +5749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151947904"/>
+        <c:crossAx val="84374592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6036,11 +6036,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161442432"/>
-        <c:axId val="164959360"/>
+        <c:axId val="84376896"/>
+        <c:axId val="132055040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161442432"/>
+        <c:axId val="84376896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6114,12 +6114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="164959360"/>
+        <c:crossAx val="132055040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164959360"/>
+        <c:axId val="132055040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6203,7 +6203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="161442432"/>
+        <c:crossAx val="84376896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6490,11 +6490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="184198272"/>
-        <c:axId val="184200576"/>
+        <c:axId val="132056768"/>
+        <c:axId val="132057344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="184198272"/>
+        <c:axId val="132056768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6568,12 +6568,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184200576"/>
+        <c:crossAx val="132057344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184200576"/>
+        <c:axId val="132057344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6657,7 +6657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184198272"/>
+        <c:crossAx val="132056768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6944,11 +6944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160392320"/>
-        <c:axId val="160394240"/>
+        <c:axId val="132059072"/>
+        <c:axId val="132059648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160392320"/>
+        <c:axId val="132059072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7022,12 +7022,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160394240"/>
+        <c:crossAx val="132059648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160394240"/>
+        <c:axId val="132059648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7111,7 +7111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160392320"/>
+        <c:crossAx val="132059072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7398,11 +7398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160403456"/>
-        <c:axId val="160405376"/>
+        <c:axId val="132061376"/>
+        <c:axId val="132061952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160403456"/>
+        <c:axId val="132061376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7476,12 +7476,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160405376"/>
+        <c:crossAx val="132061952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160405376"/>
+        <c:axId val="132061952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7565,7 +7565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160403456"/>
+        <c:crossAx val="132061376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7834,11 +7834,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160418432"/>
-        <c:axId val="160420608"/>
+        <c:axId val="132653632"/>
+        <c:axId val="132654208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160418432"/>
+        <c:axId val="132653632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7912,12 +7912,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160420608"/>
+        <c:crossAx val="132654208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160420608"/>
+        <c:axId val="132654208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8001,7 +8001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160418432"/>
+        <c:crossAx val="132653632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8288,11 +8288,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160507392"/>
-        <c:axId val="160509312"/>
+        <c:axId val="132655936"/>
+        <c:axId val="132656512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160507392"/>
+        <c:axId val="132655936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8366,12 +8366,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160509312"/>
+        <c:crossAx val="132656512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160509312"/>
+        <c:axId val="132656512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8455,7 +8455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160507392"/>
+        <c:crossAx val="132655936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8742,11 +8742,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="160637312"/>
-        <c:axId val="160639232"/>
+        <c:axId val="132658240"/>
+        <c:axId val="132658816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="160637312"/>
+        <c:axId val="132658240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8820,12 +8820,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160639232"/>
+        <c:crossAx val="132658816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160639232"/>
+        <c:axId val="132658816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8909,7 +8909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="160637312"/>
+        <c:crossAx val="132658240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13491,18 +13491,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="C20:C24"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="C25:C29"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13513,7 +13513,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13797,13 +13797,13 @@
         <v>41</v>
       </c>
       <c r="B15">
-        <v>-5.6661099999999996E-4</v>
+        <v>-1.23921E-2</v>
       </c>
       <c r="C15">
-        <v>5.2130999999999998</v>
+        <v>5.0993899999999996</v>
       </c>
       <c r="D15">
-        <v>-5.1663300000000003</v>
+        <v>-5.1171800000000003</v>
       </c>
       <c r="E15" s="73">
         <f t="shared" ref="E15:G20" si="1">E4</f>
@@ -13819,7 +13819,7 @@
       </c>
       <c r="I15">
         <f t="shared" ref="I15:I20" si="2">SLOPE(E15:G15,B15:D15)</f>
-        <v>-138.1581705135286</v>
+        <v>-140.36147276060078</v>
       </c>
       <c r="J15" s="74">
         <v>-4.8987400000000004E-3</v>
@@ -13830,13 +13830,13 @@
         <v>42</v>
       </c>
       <c r="B16">
-        <v>0.41709299999999999</v>
+        <v>4.4335300000000001E-2</v>
       </c>
       <c r="C16">
-        <v>5.1879499999999998</v>
+        <v>5.3601099999999997</v>
       </c>
       <c r="D16">
-        <v>-5.0243599999999997</v>
+        <v>-5.0779300000000003</v>
       </c>
       <c r="E16" s="73">
         <f t="shared" si="1"/>
@@ -13852,7 +13852,7 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>-143.4879360926524</v>
+        <v>-140.58796921548651</v>
       </c>
       <c r="J16" s="74">
         <v>1.4701499999999999E-2</v>
@@ -13863,13 +13863,13 @@
         <v>43</v>
       </c>
       <c r="B17">
-        <v>0.107086</v>
+        <v>-1.5067399999999999E-3</v>
       </c>
       <c r="C17">
-        <v>5.7964900000000004</v>
+        <v>5.7537200000000004</v>
       </c>
       <c r="D17">
-        <v>-5.6183699999999996</v>
+        <v>-5.7290599999999996</v>
       </c>
       <c r="E17" s="73">
         <f t="shared" si="1"/>
@@ -13885,7 +13885,7 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>-122.09233263429829</v>
+        <v>-121.37040590708075</v>
       </c>
       <c r="J17" s="74">
         <v>8.8223899999999994E-2</v>
@@ -13896,13 +13896,13 @@
         <v>44</v>
       </c>
       <c r="B18">
-        <v>-1.25734E-2</v>
+        <v>-9.0975299999999995E-2</v>
       </c>
       <c r="C18">
-        <v>5.0496499999999997</v>
+        <v>5.6192900000000003</v>
       </c>
       <c r="D18">
-        <v>-6.3145699999999998</v>
+        <v>-5.9511200000000004</v>
       </c>
       <c r="E18" s="73">
         <f t="shared" si="1"/>
@@ -13918,7 +13918,7 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>-130.23854254323442</v>
+        <v>-128.392932625301</v>
       </c>
       <c r="J18" s="74">
         <v>-5.0043700000000002E-3</v>
@@ -13929,13 +13929,13 @@
         <v>46</v>
       </c>
       <c r="B19">
-        <v>-8.4114099999999997E-2</v>
+        <v>-0.167408</v>
       </c>
       <c r="C19">
-        <v>5.5513199999999996</v>
+        <v>5.6644899999999998</v>
       </c>
       <c r="D19">
-        <v>-6.0197200000000004</v>
+        <v>-5.9615799999999997</v>
       </c>
       <c r="E19" s="73">
         <f t="shared" si="1"/>
@@ -13951,7 +13951,7 @@
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>-126.90989770087207</v>
+        <v>-126.33728381781725</v>
       </c>
       <c r="J19" s="74">
         <v>-8.8976399999999997E-2</v>
@@ -13962,13 +13962,13 @@
         <v>45</v>
       </c>
       <c r="B20">
-        <v>0.108373</v>
+        <v>0.16882800000000001</v>
       </c>
       <c r="C20">
-        <v>5.4248200000000004</v>
+        <v>5.9235600000000002</v>
       </c>
       <c r="D20">
-        <v>-5.4069599999999998</v>
+        <v>-5.5664899999999999</v>
       </c>
       <c r="E20" s="73">
         <f t="shared" si="1"/>
@@ -13984,7 +13984,7 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>-135.37403190719587</v>
+        <v>-127.63275536590128</v>
       </c>
       <c r="J20" s="74">
         <v>9.9382200000000004E-2</v>

</xml_diff>